<commit_message>
define spreadsheet tables, add and test time date module, use tk as UI module
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -1,40 +1,410 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView windowWidth="22488" windowHeight="9024" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="workers" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>check out time</t>
+  </si>
+  <si>
+    <t>chick-in time</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>張三01</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,85 +412,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -403,37 +1001,83 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>world!</t>
-        </is>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="32.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44060.6240393519</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44060.7073726832</v>
+      </c>
+      <c r="D2">
+        <f>(C2-B2)*24</f>
+        <v>1.99999995308463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>